<commit_message>
Search for img once when list components for sets
</commit_message>
<xml_diff>
--- a/search/data/Test Plan.xlsx
+++ b/search/data/Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\search\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED82455-B380-4764-ABCB-3E917D6DE37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69EB7E3-11F7-4B25-8BAB-A0CD1D1C44D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3408" yWindow="0" windowWidth="17280" windowHeight="12360" xr2:uid="{2D681D24-791C-4F0F-A932-3C86F5FC259D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Test</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Popup: "Search returned no components"</t>
+  </si>
+  <si>
+    <t>search for component</t>
+  </si>
+  <si>
+    <t>verify image in component table only searched once</t>
   </si>
 </sst>
 </file>
@@ -472,17 +478,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C82714B2-64B0-491F-9BD1-83B74FAE943A}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="4.15625" style="2" customWidth="1"/>
     <col min="2" max="2" width="23.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.3125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.05078125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -617,6 +624,17 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>